<commit_message>
work session before video recording
- add time series plots
- fix wind direction calculation (rotated 180 deg)
- update ppt slides and final report
</commit_message>
<xml_diff>
--- a/data_siteH_LLJs/LLJ_summary.xlsx
+++ b/data_siteH_LLJs/LLJ_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexhirst/Documents/CU Boulder/ATOC 5770/project/data_siteH_LLJs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760E57D4-6FE2-9F41-911D-27BF84252909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E0CCE1-B8DB-8A4C-985E-3938F6A99595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="4100" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Time</t>
+    <t>Time (UTC)</t>
   </si>
   <si>
     <t>LLJ class</t>
@@ -40,7 +40,7 @@
     <t>Nose Windspeed [m/s]</t>
   </si>
   <si>
-    <t>Nose Wind Direction [deg]</t>
+    <t>Nose Wind Direction [rad]</t>
   </si>
 </sst>
 </file>
@@ -100,7 +100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -108,6 +108,7 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,19 +413,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G355"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="A198" sqref="A198:G200"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E213" sqref="E213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.1640625" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="34" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -567,20 +568,20 @@
       <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="3">
         <v>454.6633369868303</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="3">
         <v>4.6018087774405387</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="3">
         <v>10.55404498555056</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="3">
         <v>12.952829995315399</v>
       </c>
-      <c r="G24">
-        <v>176.7562436142818</v>
+      <c r="G24" s="3">
+        <v>-3.2437563857182279</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -590,20 +591,20 @@
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="3">
         <v>532.60562332742984</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="3">
         <v>3.8670467318452482</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="3">
         <v>12.0794520409996</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="3">
         <v>15.415565210635309</v>
       </c>
-      <c r="G25">
-        <v>180.7124451314067</v>
+      <c r="G25" s="3">
+        <v>0.71244513140669596</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -613,20 +614,20 @@
       <c r="B26">
         <v>2</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="3">
         <v>558.586385440963</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="3">
         <v>6.025352242090845</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="3">
         <v>16.347173956844198</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="3">
         <v>18.070302739790939</v>
       </c>
-      <c r="G26">
-        <v>196.5659101300007</v>
+      <c r="G26" s="3">
+        <v>16.565910130000731</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -636,20 +637,20 @@
       <c r="B27">
         <v>2</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="3">
         <v>558.586385440963</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="3">
         <v>7.4956101342775554</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="3">
         <v>15.88868940845729</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="3">
         <v>18.580057140023339</v>
       </c>
-      <c r="G27">
-        <v>194.13417380679061</v>
+      <c r="G27" s="3">
+        <v>14.13417380679056</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -659,20 +660,20 @@
       <c r="B28">
         <v>2</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="3">
         <v>584.56714755449616</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="3">
         <v>9.8221152163769823</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="3">
         <v>13.426025053201769</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="3">
         <v>19.02541787480946</v>
       </c>
-      <c r="G28">
-        <v>203.68720443889279</v>
+      <c r="G28" s="3">
+        <v>23.687204438892788</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -682,20 +683,20 @@
       <c r="B29">
         <v>2</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="3">
         <v>636.52867178156248</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="3">
         <v>8.7176890582110715</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="3">
         <v>13.16037806813725</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="3">
         <v>19.11994452444134</v>
       </c>
-      <c r="G29">
-        <v>199.9794563168677</v>
+      <c r="G29" s="3">
+        <v>19.979456316867669</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -705,20 +706,20 @@
       <c r="B30">
         <v>2</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="3">
         <v>558.586385440963</v>
       </c>
-      <c r="D30">
-        <v>8.6319514397602592</v>
-      </c>
-      <c r="E30">
+      <c r="D30" s="3">
+        <v>8.6319514397602646</v>
+      </c>
+      <c r="E30" s="3">
         <v>10.2560052854134</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="3">
         <v>19.72596607417977</v>
       </c>
-      <c r="G30">
-        <v>200.95982098399429</v>
+      <c r="G30" s="3">
+        <v>20.959820983994259</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -728,20 +729,20 @@
       <c r="B31">
         <v>3</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="3">
         <v>610.54790966802932</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="3">
         <v>9.7172456510646548</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="3">
         <v>10.56671086257089</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="3">
         <v>20.886896148392569</v>
       </c>
-      <c r="G31">
-        <v>199.79558674035451</v>
+      <c r="G31" s="3">
+        <v>19.795586740354508</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -751,20 +752,20 @@
       <c r="B32">
         <v>3</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="3">
         <v>636.52867178156248</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="3">
         <v>12.483392432562569</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="3">
         <v>12.42361126315056</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="3">
         <v>23.052401823882558</v>
       </c>
-      <c r="G32">
-        <v>205.92178270637649</v>
+      <c r="G32" s="3">
+        <v>25.92178270637655</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -774,20 +775,20 @@
       <c r="B33">
         <v>3</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="3">
         <v>662.50943389509564</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="3">
         <v>12.85571116222685</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="3">
         <v>10.72432556916633</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="3">
         <v>22.29127604471342</v>
       </c>
-      <c r="G33">
-        <v>203.65172741379789</v>
+      <c r="G33" s="3">
+        <v>23.651727413797939</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -797,541 +798,1061 @@
       <c r="B34">
         <v>3</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="3">
         <v>688.4901960086288</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="3">
         <v>13.10932580015721</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="3">
         <v>10.690201531166551</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="3">
         <v>21.757832841762148</v>
       </c>
-      <c r="G34">
-        <v>202.9095342028661</v>
+      <c r="G34" s="3">
+        <v>22.909534202866102</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>44876.145871063069</v>
       </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>44876.166907290622</v>
       </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>44876.187534610428</v>
       </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>44876.208571175732</v>
       </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>44876.229200343289</v>
       </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>44876.250244100876</v>
       </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>44876.270874420799</v>
       </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>44876.291911105312</v>
       </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>44876.312536795929</v>
       </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>44876.333569208771</v>
       </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44876.354210774087</v>
       </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>44876.375240842499</v>
       </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>44876.395867824547</v>
       </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>44876.416906118393</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>44876.437541206673</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>44876.458576838173</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>44876.479201038674</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>44876.500244220093</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>44876.520876288399</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>44876.54190810521</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>44876.562534014367</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>44876.583570122712</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>44876.604202191033</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>44876.625241994851</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>44876.64587672551</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>44876.666906118393</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>44876.687537352227</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>44876.708579381288</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>44876.729207833603</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>44876.75024517376</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>44876.770874738679</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>44876.791908661507</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>44876.812540531158</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>44876.833581447587</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>44876.854208707802</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>44876.875238100693</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>44876.895874500267</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>44876.916915496178</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>44876.937533537537</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>44876.958580891282</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>44876.979201237351</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>44877.000239236237</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>44877.020868517291</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>44877.041913424917</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>44877.062540278159</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>44877.083580096572</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>44877.104204515606</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>44877.125242243208</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>44877.145868052372</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>44877.166906356797</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>44877.187536696583</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>44877.208571056522</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>44877.229208687939</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>44877.250242710114</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>44877.270866195358</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>44877.291904290512</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>44877.312543869019</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>44877.333575805023</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>44877.354201753922</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>44877.375242829323</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>44877.39586631456</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>44877.416908899941</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>44877.437536795929</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>44877.458575248718</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
+      <c r="G98" s="3"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>44877.479200800262</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+      <c r="G99" s="3"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>44877.50024072329</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="3"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>44877.520866195358</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>44877.541906237588</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>44877.56254410743</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>44877.583574533463</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>44877.60420266787</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>44877.625241438538</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="3"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>44877.645875334732</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="3"/>
+      <c r="F107" s="3"/>
+      <c r="G107" s="3"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>44877.666912714631</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+      <c r="G108" s="3"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>44877.687537352227</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="3"/>
+      <c r="F109" s="3"/>
+      <c r="G109" s="3"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>44877.708571513482</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="3"/>
+      <c r="F110" s="3"/>
+      <c r="G110" s="3"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>44877.729203383133</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
+      <c r="E111" s="3"/>
+      <c r="F111" s="3"/>
+      <c r="G111" s="3"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>44877.750239610672</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="3"/>
+      <c r="G112" s="3"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>44877.770875453949</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
+      <c r="E113" s="3"/>
+      <c r="F113" s="3"/>
+      <c r="G113" s="3"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>44877.791902542107</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
+      <c r="E114" s="3"/>
+      <c r="F114" s="3"/>
+      <c r="G114" s="3"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>44877.81253973642</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
+      <c r="E115" s="3"/>
+      <c r="F115" s="3"/>
+      <c r="G115" s="3"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>44877.83357548713</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C116" s="3"/>
+      <c r="D116" s="3"/>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3"/>
+      <c r="G116" s="3"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>44877.854205767297</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
+      <c r="E117" s="3"/>
+      <c r="F117" s="3"/>
+      <c r="G117" s="3"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>44877.875248750053</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3"/>
+      <c r="F118" s="3"/>
+      <c r="G118" s="3"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>44877.895874500267</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C119" s="3"/>
+      <c r="D119" s="3"/>
+      <c r="E119" s="3"/>
+      <c r="F119" s="3"/>
+      <c r="G119" s="3"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>44877.916908899941</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C120" s="3"/>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="3"/>
+      <c r="G120" s="3"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>44877.937535524361</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
+      <c r="E121" s="3"/>
+      <c r="F121" s="3"/>
+      <c r="G121" s="3"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>44877.958575089768</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3"/>
+      <c r="F122" s="3"/>
+      <c r="G122" s="3"/>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>44877.979201952607</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3"/>
+      <c r="F123" s="3"/>
+      <c r="G123" s="3"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>44878.000240972113</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C124" s="3"/>
+      <c r="D124" s="3"/>
+      <c r="E124" s="3"/>
+      <c r="F124" s="3"/>
+      <c r="G124" s="3"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>44878.020875695009</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C125" s="3"/>
+      <c r="D125" s="3"/>
+      <c r="E125" s="3"/>
+      <c r="F125" s="3"/>
+      <c r="G125" s="3"/>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>44878.041910534099</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="3"/>
+      <c r="G126" s="3"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>44878.06253576278</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C127" s="3"/>
+      <c r="D127" s="3"/>
+      <c r="E127" s="3"/>
+      <c r="F127" s="3"/>
+      <c r="G127" s="3"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>44878.083574076503</v>
       </c>
+      <c r="C128" s="3"/>
+      <c r="D128" s="3"/>
+      <c r="E128" s="3"/>
+      <c r="F128" s="3"/>
+      <c r="G128" s="3"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>44878.104209491932</v>
       </c>
+      <c r="C129" s="3"/>
+      <c r="D129" s="3"/>
+      <c r="E129" s="3"/>
+      <c r="F129" s="3"/>
+      <c r="G129" s="3"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>44878.125247915581</v>
       </c>
+      <c r="C130" s="3"/>
+      <c r="D130" s="3"/>
+      <c r="E130" s="3"/>
+      <c r="F130" s="3"/>
+      <c r="G130" s="3"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>44878.145868519932</v>
       </c>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
+      <c r="E131" s="3"/>
+      <c r="F131" s="3"/>
+      <c r="G131" s="3"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>44878.166906356797</v>
       </c>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="3"/>
+      <c r="G132" s="3"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>44878.187536915138</v>
       </c>
+      <c r="C133" s="3"/>
+      <c r="D133" s="3"/>
+      <c r="E133" s="3"/>
+      <c r="F133" s="3"/>
+      <c r="G133" s="3"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>44878.208576619618</v>
       </c>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
+      <c r="E134" s="3"/>
+      <c r="F134" s="3"/>
+      <c r="G134" s="3"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
         <v>44878.22920149564</v>
       </c>
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
+      <c r="E135" s="3"/>
+      <c r="F135" s="3"/>
+      <c r="G135" s="3"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>44878.250243981682</v>
       </c>
+      <c r="C136" s="3"/>
+      <c r="D136" s="3"/>
+      <c r="E136" s="3"/>
+      <c r="F136" s="3"/>
+      <c r="G136" s="3"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
         <v>44878.270871520042</v>
       </c>
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
+      <c r="E137" s="3"/>
+      <c r="F137" s="3"/>
+      <c r="G137" s="3"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>44878.291909714528</v>
       </c>
+      <c r="C138" s="3"/>
+      <c r="D138" s="3"/>
+      <c r="E138" s="3"/>
+      <c r="F138" s="3"/>
+      <c r="G138" s="3"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
@@ -1340,20 +1861,20 @@
       <c r="B139">
         <v>0</v>
       </c>
-      <c r="C139">
+      <c r="C139" s="3">
         <v>142.89419162443241</v>
       </c>
-      <c r="D139">
+      <c r="D139" s="3">
         <v>1.682225046832009</v>
       </c>
-      <c r="E139">
+      <c r="E139" s="3">
         <v>7.3806495284679032</v>
       </c>
-      <c r="F139">
+      <c r="F139" s="3">
         <v>10.59391871428871</v>
       </c>
-      <c r="G139">
-        <v>286.55867388814181</v>
+      <c r="G139" s="3">
+        <v>106.5586738881418</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
@@ -1363,26 +1884,31 @@
       <c r="B140">
         <v>0</v>
       </c>
-      <c r="C140">
+      <c r="C140" s="3">
         <v>168.87495373796551</v>
       </c>
-      <c r="D140">
+      <c r="D140" s="3">
         <v>2.571314527156356</v>
       </c>
-      <c r="E140">
+      <c r="E140" s="3">
         <v>6.2867731478394724</v>
       </c>
-      <c r="F140">
+      <c r="F140" s="3">
         <v>10.15243508521621</v>
       </c>
-      <c r="G140">
-        <v>296.64057711265423</v>
+      <c r="G140" s="3">
+        <v>116.6405771126542</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
         <v>44878.354204614952</v>
       </c>
+      <c r="C141" s="3"/>
+      <c r="D141" s="3"/>
+      <c r="E141" s="3"/>
+      <c r="F141" s="3"/>
+      <c r="G141" s="3"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
@@ -1391,20 +1917,20 @@
       <c r="B142">
         <v>0</v>
       </c>
-      <c r="C142">
+      <c r="C142" s="3">
         <v>168.87495373796551</v>
       </c>
-      <c r="D142">
+      <c r="D142" s="3">
         <v>3.375974003861494</v>
       </c>
-      <c r="E142">
+      <c r="E142" s="3">
         <v>5.5482150696822927</v>
       </c>
-      <c r="F142">
+      <c r="F142" s="3">
         <v>10.26635964532076</v>
       </c>
-      <c r="G142">
-        <v>300.19121654765598</v>
+      <c r="G142" s="3">
+        <v>120.191216547656</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
@@ -1414,41 +1940,61 @@
       <c r="B143">
         <v>0</v>
       </c>
-      <c r="C143">
+      <c r="C143" s="3">
         <v>168.87495373796551</v>
       </c>
-      <c r="D143">
+      <c r="D143" s="3">
         <v>3.4429921055656338</v>
       </c>
-      <c r="E143">
+      <c r="E143" s="3">
         <v>5.2086502801057417</v>
       </c>
-      <c r="F143">
+      <c r="F143" s="3">
         <v>10.253047901174529</v>
       </c>
-      <c r="G143">
-        <v>303.60541422510818</v>
+      <c r="G143" s="3">
+        <v>123.60541422510821</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
         <v>44878.416901985802</v>
       </c>
+      <c r="C144" s="3"/>
+      <c r="D144" s="3"/>
+      <c r="E144" s="3"/>
+      <c r="F144" s="3"/>
+      <c r="G144" s="3"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
         <v>44878.437541762993</v>
       </c>
+      <c r="C145" s="3"/>
+      <c r="D145" s="3"/>
+      <c r="E145" s="3"/>
+      <c r="F145" s="3"/>
+      <c r="G145" s="3"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>44878.458576639488</v>
       </c>
+      <c r="C146" s="3"/>
+      <c r="D146" s="3"/>
+      <c r="E146" s="3"/>
+      <c r="F146" s="3"/>
+      <c r="G146" s="3"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
         <v>44878.479206601769</v>
       </c>
+      <c r="C147" s="3"/>
+      <c r="D147" s="3"/>
+      <c r="E147" s="3"/>
+      <c r="F147" s="3"/>
+      <c r="G147" s="3"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
@@ -1457,266 +2003,511 @@
       <c r="B148">
         <v>0</v>
       </c>
-      <c r="C148">
+      <c r="C148" s="3">
         <v>168.87495373796551</v>
       </c>
-      <c r="D148">
+      <c r="D148" s="3">
         <v>7.896632322947724</v>
       </c>
-      <c r="E148">
+      <c r="E148" s="3">
         <v>5.3201731776244241</v>
       </c>
-      <c r="F148">
+      <c r="F148" s="3">
         <v>11.952285747796321</v>
       </c>
-      <c r="G148">
-        <v>308.43199532647259</v>
+      <c r="G148" s="3">
+        <v>128.43199532647259</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
         <v>44878.520871996872</v>
       </c>
+      <c r="C149" s="3"/>
+      <c r="D149" s="3"/>
+      <c r="E149" s="3"/>
+      <c r="F149" s="3"/>
+      <c r="G149" s="3"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
         <v>44878.541900595017</v>
       </c>
+      <c r="C150" s="3"/>
+      <c r="D150" s="3"/>
+      <c r="E150" s="3"/>
+      <c r="F150" s="3"/>
+      <c r="G150" s="3"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
         <v>44878.562537829072</v>
       </c>
+      <c r="C151" s="3"/>
+      <c r="D151" s="3"/>
+      <c r="E151" s="3"/>
+      <c r="F151" s="3"/>
+      <c r="G151" s="3"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
         <v>44878.583573977143</v>
       </c>
+      <c r="C152" s="3"/>
+      <c r="D152" s="3"/>
+      <c r="E152" s="3"/>
+      <c r="F152" s="3"/>
+      <c r="G152" s="3"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
         <v>44878.604209264107</v>
       </c>
+      <c r="C153" s="3"/>
+      <c r="D153" s="3"/>
+      <c r="E153" s="3"/>
+      <c r="F153" s="3"/>
+      <c r="G153" s="3"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
         <v>44878.625237623841</v>
       </c>
+      <c r="C154" s="3"/>
+      <c r="D154" s="3"/>
+      <c r="E154" s="3"/>
+      <c r="F154" s="3"/>
+      <c r="G154" s="3"/>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
         <v>44878.645869572953</v>
       </c>
+      <c r="C155" s="3"/>
+      <c r="D155" s="3"/>
+      <c r="E155" s="3"/>
+      <c r="F155" s="3"/>
+      <c r="G155" s="3"/>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
         <v>44878.666908661507</v>
       </c>
+      <c r="C156" s="3"/>
+      <c r="D156" s="3"/>
+      <c r="E156" s="3"/>
+      <c r="F156" s="3"/>
+      <c r="G156" s="3"/>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
         <v>44878.687540849038</v>
       </c>
+      <c r="C157" s="3"/>
+      <c r="D157" s="3"/>
+      <c r="E157" s="3"/>
+      <c r="F157" s="3"/>
+      <c r="G157" s="3"/>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
         <v>44878.708576997124</v>
       </c>
+      <c r="C158" s="3"/>
+      <c r="D158" s="3"/>
+      <c r="E158" s="3"/>
+      <c r="F158" s="3"/>
+      <c r="G158" s="3"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
         <v>44878.729202429437</v>
       </c>
+      <c r="C159" s="3"/>
+      <c r="D159" s="3"/>
+      <c r="E159" s="3"/>
+      <c r="F159" s="3"/>
+      <c r="G159" s="3"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
         <v>44878.750247240059</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C160" s="3"/>
+      <c r="D160" s="3"/>
+      <c r="E160" s="3"/>
+      <c r="F160" s="3"/>
+      <c r="G160" s="3"/>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" s="2">
         <v>44878.770876963921</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C161" s="3"/>
+      <c r="D161" s="3"/>
+      <c r="E161" s="3"/>
+      <c r="F161" s="3"/>
+      <c r="G161" s="3"/>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
         <v>44878.791912396751</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C162" s="3"/>
+      <c r="D162" s="3"/>
+      <c r="E162" s="3"/>
+      <c r="F162" s="3"/>
+      <c r="G162" s="3"/>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="2">
         <v>44878.81253369648</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C163" s="3"/>
+      <c r="D163" s="3"/>
+      <c r="E163" s="3"/>
+      <c r="F163" s="3"/>
+      <c r="G163" s="3"/>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
         <v>44878.833573341362</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C164" s="3"/>
+      <c r="D164" s="3"/>
+      <c r="E164" s="3"/>
+      <c r="F164" s="3"/>
+      <c r="G164" s="3"/>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
         <v>44878.85420497258</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C165" s="3"/>
+      <c r="D165" s="3"/>
+      <c r="E165" s="3"/>
+      <c r="F165" s="3"/>
+      <c r="G165" s="3"/>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" s="2">
         <v>44878.875239133828</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C166" s="3"/>
+      <c r="D166" s="3"/>
+      <c r="E166" s="3"/>
+      <c r="F166" s="3"/>
+      <c r="G166" s="3"/>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" s="2">
         <v>44878.895871082939</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C167" s="3"/>
+      <c r="D167" s="3"/>
+      <c r="E167" s="3"/>
+      <c r="F167" s="3"/>
+      <c r="G167" s="3"/>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" s="2">
         <v>44878.916912635163</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C168" s="3"/>
+      <c r="D168" s="3"/>
+      <c r="E168" s="3"/>
+      <c r="F168" s="3"/>
+      <c r="G168" s="3"/>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" s="2">
         <v>44878.937538305923</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C169" s="3"/>
+      <c r="D169" s="3"/>
+      <c r="E169" s="3"/>
+      <c r="F169" s="3"/>
+      <c r="G169" s="3"/>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
         <v>44878.958574771867</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C170" s="3"/>
+      <c r="D170" s="3"/>
+      <c r="E170" s="3"/>
+      <c r="F170" s="3"/>
+      <c r="G170" s="3"/>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" s="2">
         <v>44878.979208787277</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C171" s="3"/>
+      <c r="D171" s="3"/>
+      <c r="E171" s="3"/>
+      <c r="F171" s="3"/>
+      <c r="G171" s="3"/>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
         <v>44879.000239004548</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C172" s="3"/>
+      <c r="D172" s="3"/>
+      <c r="E172" s="3"/>
+      <c r="F172" s="3"/>
+      <c r="G172" s="3"/>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" s="2">
         <v>44879.020869096108</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C173" s="3"/>
+      <c r="D173" s="3"/>
+      <c r="E173" s="3"/>
+      <c r="F173" s="3"/>
+      <c r="G173" s="3"/>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
         <v>44879.041914582253</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C174" s="3"/>
+      <c r="D174" s="3"/>
+      <c r="E174" s="3"/>
+      <c r="F174" s="3"/>
+      <c r="G174" s="3"/>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" s="2">
         <v>44879.06253912051</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C175" s="3"/>
+      <c r="D175" s="3"/>
+      <c r="E175" s="3"/>
+      <c r="F175" s="3"/>
+      <c r="G175" s="3"/>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" s="2">
         <v>44879.083582987383</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C176" s="3"/>
+      <c r="D176" s="3"/>
+      <c r="E176" s="3"/>
+      <c r="F176" s="3"/>
+      <c r="G176" s="3"/>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" s="2">
         <v>44879.10420694881</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C177" s="3"/>
+      <c r="D177" s="3"/>
+      <c r="E177" s="3"/>
+      <c r="F177" s="3"/>
+      <c r="G177" s="3"/>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" s="2">
         <v>44879.125241438538</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C178" s="3"/>
+      <c r="D178" s="3"/>
+      <c r="E178" s="3"/>
+      <c r="F178" s="3"/>
+      <c r="G178" s="3"/>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" s="2">
         <v>44879.145869791508</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C179" s="3"/>
+      <c r="D179" s="3"/>
+      <c r="E179" s="3"/>
+      <c r="F179" s="3"/>
+      <c r="G179" s="3"/>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" s="2">
         <v>44879.166906595223</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C180" s="3"/>
+      <c r="D180" s="3"/>
+      <c r="E180" s="3"/>
+      <c r="F180" s="3"/>
+      <c r="G180" s="3"/>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" s="2">
         <v>44879.187537391983</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C181" s="3"/>
+      <c r="D181" s="3"/>
+      <c r="E181" s="3"/>
+      <c r="F181" s="3"/>
+      <c r="G181" s="3"/>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" s="2">
         <v>44879.208575348057</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C182" s="3"/>
+      <c r="D182" s="3"/>
+      <c r="E182" s="3"/>
+      <c r="F182" s="3"/>
+      <c r="G182" s="3"/>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" s="2">
         <v>44879.229209721088</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C183" s="3"/>
+      <c r="D183" s="3"/>
+      <c r="E183" s="3"/>
+      <c r="F183" s="3"/>
+      <c r="G183" s="3"/>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
         <v>44879.250241657093</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C184" s="3"/>
+      <c r="D184" s="3"/>
+      <c r="E184" s="3"/>
+      <c r="F184" s="3"/>
+      <c r="G184" s="3"/>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" s="2">
         <v>44879.270870486893</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C185" s="3"/>
+      <c r="D185" s="3"/>
+      <c r="E185" s="3"/>
+      <c r="F185" s="3"/>
+      <c r="G185" s="3"/>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" s="2">
         <v>44879.291907290622</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C186" s="3"/>
+      <c r="D186" s="3"/>
+      <c r="E186" s="3"/>
+      <c r="F186" s="3"/>
+      <c r="G186" s="3"/>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" s="2">
         <v>44879.312542120613</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C187" s="3"/>
+      <c r="D187" s="3"/>
+      <c r="E187" s="3"/>
+      <c r="F187" s="3"/>
+      <c r="G187" s="3"/>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
         <v>44879.333576043427</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C188" s="3"/>
+      <c r="D188" s="3"/>
+      <c r="E188" s="3"/>
+      <c r="F188" s="3"/>
+      <c r="G188" s="3"/>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" s="2">
         <v>44879.354203581803</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C189" s="3"/>
+      <c r="D189" s="3"/>
+      <c r="E189" s="3"/>
+      <c r="F189" s="3"/>
+      <c r="G189" s="3"/>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" s="2">
         <v>44879.375236233071</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C190" s="3"/>
+      <c r="D190" s="3"/>
+      <c r="E190" s="3"/>
+      <c r="F190" s="3"/>
+      <c r="G190" s="3"/>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" s="2">
         <v>44879.39587338765</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C191" s="3"/>
+      <c r="D191" s="3"/>
+      <c r="E191" s="3"/>
+      <c r="F191" s="3"/>
+      <c r="G191" s="3"/>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" s="2">
         <v>44879.416910052292</v>
       </c>
+      <c r="C192" s="3"/>
+      <c r="D192" s="3"/>
+      <c r="E192" s="3"/>
+      <c r="F192" s="3"/>
+      <c r="G192" s="3"/>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" s="2">
         <v>44879.437543869019</v>
       </c>
+      <c r="C193" s="3"/>
+      <c r="D193" s="3"/>
+      <c r="E193" s="3"/>
+      <c r="F193" s="3"/>
+      <c r="G193" s="3"/>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
         <v>44879.458574652657</v>
       </c>
+      <c r="C194" s="3"/>
+      <c r="D194" s="3"/>
+      <c r="E194" s="3"/>
+      <c r="F194" s="3"/>
+      <c r="G194" s="3"/>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195" s="2">
         <v>44879.479206720993</v>
       </c>
+      <c r="C195" s="3"/>
+      <c r="D195" s="3"/>
+      <c r="E195" s="3"/>
+      <c r="F195" s="3"/>
+      <c r="G195" s="3"/>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196" s="2">
         <v>44879.500243624047</v>
       </c>
+      <c r="C196" s="3"/>
+      <c r="D196" s="3"/>
+      <c r="E196" s="3"/>
+      <c r="F196" s="3"/>
+      <c r="G196" s="3"/>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197" s="2">
         <v>44879.520874063172</v>
       </c>
+      <c r="C197" s="3"/>
+      <c r="D197" s="3"/>
+      <c r="E197" s="3"/>
+      <c r="F197" s="3"/>
+      <c r="G197" s="3"/>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198" s="2">
@@ -1725,20 +2516,20 @@
       <c r="B198">
         <v>0</v>
       </c>
-      <c r="C198">
+      <c r="C198" s="3">
         <v>532.60562332742984</v>
       </c>
-      <c r="D198">
+      <c r="D198" s="3">
         <v>5.6738648403125334</v>
       </c>
-      <c r="E198">
+      <c r="E198" s="3">
         <v>5.535199332135436</v>
       </c>
-      <c r="F198">
+      <c r="F198" s="3">
         <v>13.854729682886109</v>
       </c>
-      <c r="G198">
-        <v>360.7405743782287</v>
+      <c r="G198" s="3">
+        <v>180.7405743782287</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.2">
@@ -1748,20 +2539,20 @@
       <c r="B199">
         <v>1</v>
       </c>
-      <c r="C199">
+      <c r="C199" s="3">
         <v>480.64409910036352</v>
       </c>
-      <c r="D199">
+      <c r="D199" s="3">
         <v>4.431470820636795</v>
       </c>
-      <c r="E199">
+      <c r="E199" s="3">
         <v>6.5306750164267493</v>
       </c>
-      <c r="F199">
+      <c r="F199" s="3">
         <v>12.49415735437584</v>
       </c>
-      <c r="G199">
-        <v>348.51966476513292</v>
+      <c r="G199" s="3">
+        <v>168.51966476513289</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.2">
@@ -1771,796 +2562,1571 @@
       <c r="B200">
         <v>1</v>
       </c>
-      <c r="C200">
+      <c r="C200" s="3">
         <v>532.60562332742984</v>
       </c>
-      <c r="D200">
+      <c r="D200" s="3">
         <v>6.1683028445985268</v>
       </c>
-      <c r="E200">
+      <c r="E200" s="3">
         <v>6.3751964825544727</v>
       </c>
-      <c r="F200">
+      <c r="F200" s="3">
         <v>13.41622806017641</v>
       </c>
-      <c r="G200">
-        <v>355.30743780046981</v>
+      <c r="G200" s="3">
+        <v>175.30743780046981</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201" s="2">
         <v>44879.604206363358</v>
       </c>
+      <c r="C201" s="3"/>
+      <c r="D201" s="3"/>
+      <c r="E201" s="3"/>
+      <c r="F201" s="3"/>
+      <c r="G201" s="3"/>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202" s="2">
         <v>44879.625242471688</v>
       </c>
+      <c r="C202" s="3"/>
+      <c r="D202" s="3"/>
+      <c r="E202" s="3"/>
+      <c r="F202" s="3"/>
+      <c r="G202" s="3"/>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203" s="2">
         <v>44879.64586631456</v>
       </c>
+      <c r="C203" s="3"/>
+      <c r="D203" s="3"/>
+      <c r="E203" s="3"/>
+      <c r="F203" s="3"/>
+      <c r="G203" s="3"/>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204" s="2">
         <v>44879.666909456253</v>
       </c>
+      <c r="C204" s="3"/>
+      <c r="D204" s="3"/>
+      <c r="E204" s="3"/>
+      <c r="F204" s="3"/>
+      <c r="G204" s="3"/>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205" s="2">
         <v>44879.687533934914</v>
       </c>
+      <c r="C205" s="3"/>
+      <c r="D205" s="3"/>
+      <c r="E205" s="3"/>
+      <c r="F205" s="3"/>
+      <c r="G205" s="3"/>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206" s="2">
         <v>44879.708570957177</v>
       </c>
+      <c r="C206" s="3"/>
+      <c r="D206" s="3"/>
+      <c r="E206" s="3"/>
+      <c r="F206" s="3"/>
+      <c r="G206" s="3"/>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207" s="2">
         <v>44879.72920497258</v>
       </c>
+      <c r="C207" s="3"/>
+      <c r="D207" s="3"/>
+      <c r="E207" s="3"/>
+      <c r="F207" s="3"/>
+      <c r="G207" s="3"/>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208" s="2">
         <v>44879.750244061142</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C208" s="3"/>
+      <c r="D208" s="3"/>
+      <c r="E208" s="3"/>
+      <c r="F208" s="3"/>
+      <c r="G208" s="3"/>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209" s="2">
         <v>44879.770873626068</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C209" s="3"/>
+      <c r="D209" s="3"/>
+      <c r="E209" s="3"/>
+      <c r="F209" s="3"/>
+      <c r="G209" s="3"/>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210" s="2">
         <v>44879.791906038903</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C210" s="3"/>
+      <c r="D210" s="3"/>
+      <c r="E210" s="3"/>
+      <c r="F210" s="3"/>
+      <c r="G210" s="3"/>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211" s="2">
         <v>44879.8125342528</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C211" s="3"/>
+      <c r="D211" s="3"/>
+      <c r="E211" s="3"/>
+      <c r="F211" s="3"/>
+      <c r="G211" s="3"/>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A212" s="2">
         <v>44879.833575725541</v>
       </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C212" s="3"/>
+      <c r="D212" s="3"/>
+      <c r="E212" s="3"/>
+      <c r="F212" s="3"/>
+      <c r="G212" s="3"/>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A213" s="2">
         <v>44879.854208469384</v>
       </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C213" s="3"/>
+      <c r="D213" s="3"/>
+      <c r="E213" s="3"/>
+      <c r="F213" s="3"/>
+      <c r="G213" s="3"/>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A214" s="2">
         <v>44879.875239610672</v>
       </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C214" s="3"/>
+      <c r="D214" s="3"/>
+      <c r="E214" s="3"/>
+      <c r="F214" s="3"/>
+      <c r="G214" s="3"/>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A215" s="2">
         <v>44879.895871559769</v>
       </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C215" s="3"/>
+      <c r="D215" s="3"/>
+      <c r="E215" s="3"/>
+      <c r="F215" s="3"/>
+      <c r="G215" s="3"/>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216" s="2">
         <v>44879.916913191468</v>
       </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C216" s="3"/>
+      <c r="D216" s="3"/>
+      <c r="E216" s="3"/>
+      <c r="F216" s="3"/>
+      <c r="G216" s="3"/>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217" s="2">
         <v>44879.93754307428</v>
       </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C217" s="3"/>
+      <c r="D217" s="3"/>
+      <c r="E217" s="3"/>
+      <c r="F217" s="3"/>
+      <c r="G217" s="3"/>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218" s="2">
         <v>44879.958573023483</v>
       </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C218" s="3"/>
+      <c r="D218" s="3"/>
+      <c r="E218" s="3"/>
+      <c r="F218" s="3"/>
+      <c r="G218" s="3"/>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A219" s="2">
         <v>44879.979206959397</v>
       </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C219" s="3"/>
+      <c r="D219" s="3"/>
+      <c r="E219" s="3"/>
+      <c r="F219" s="3"/>
+      <c r="G219" s="3"/>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A220" s="2">
         <v>44880.000242013753</v>
       </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C220" s="3"/>
+      <c r="D220" s="3"/>
+      <c r="E220" s="3"/>
+      <c r="F220" s="3"/>
+      <c r="G220" s="3"/>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A221" s="2">
         <v>44880.020872802197</v>
       </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C221" s="3"/>
+      <c r="D221" s="3"/>
+      <c r="E221" s="3"/>
+      <c r="F221" s="3"/>
+      <c r="G221" s="3"/>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A222" s="2">
         <v>44880.041910996028</v>
       </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C222" s="3"/>
+      <c r="D222" s="3"/>
+      <c r="E222" s="3"/>
+      <c r="F222" s="3"/>
+      <c r="G222" s="3"/>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A223" s="2">
         <v>44880.062539234423</v>
       </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C223" s="3"/>
+      <c r="D223" s="3"/>
+      <c r="E223" s="3"/>
+      <c r="F223" s="3"/>
+      <c r="G223" s="3"/>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A224" s="2">
         <v>44880.083570251853</v>
       </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C224" s="3"/>
+      <c r="D224" s="3"/>
+      <c r="E224" s="3"/>
+      <c r="F224" s="3"/>
+      <c r="G224" s="3"/>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225" s="2">
         <v>44880.104203701019</v>
       </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C225" s="3"/>
+      <c r="D225" s="3"/>
+      <c r="E225" s="3"/>
+      <c r="F225" s="3"/>
+      <c r="G225" s="3"/>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226" s="2">
         <v>44880.125239471578</v>
       </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C226" s="3"/>
+      <c r="D226" s="3"/>
+      <c r="E226" s="3"/>
+      <c r="F226" s="3"/>
+      <c r="G226" s="3"/>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227" s="2">
         <v>44880.145867705338</v>
       </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C227" s="3"/>
+      <c r="D227" s="3"/>
+      <c r="E227" s="3"/>
+      <c r="F227" s="3"/>
+      <c r="G227" s="3"/>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228" s="2">
         <v>44880.166913648427</v>
       </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C228" s="3"/>
+      <c r="D228" s="3"/>
+      <c r="E228" s="3"/>
+      <c r="F228" s="3"/>
+      <c r="G228" s="3"/>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A229" s="2">
         <v>44880.187535067387</v>
       </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C229" s="3"/>
+      <c r="D229" s="3"/>
+      <c r="E229" s="3"/>
+      <c r="F229" s="3"/>
+      <c r="G229" s="3"/>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230" s="2">
         <v>44880.208578129597</v>
       </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C230" s="3"/>
+      <c r="D230" s="3"/>
+      <c r="E230" s="3"/>
+      <c r="F230" s="3"/>
+      <c r="G230" s="3"/>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A231" s="2">
         <v>44880.229210416474</v>
       </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C231" s="3"/>
+      <c r="D231" s="3"/>
+      <c r="E231" s="3"/>
+      <c r="F231" s="3"/>
+      <c r="G231" s="3"/>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A232" s="2">
         <v>44880.250237623841</v>
       </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C232" s="3"/>
+      <c r="D232" s="3"/>
+      <c r="E232" s="3"/>
+      <c r="F232" s="3"/>
+      <c r="G232" s="3"/>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233" s="2">
         <v>44880.27087233463</v>
       </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C233" s="3"/>
+      <c r="D233" s="3"/>
+      <c r="E233" s="3"/>
+      <c r="F233" s="3"/>
+      <c r="G233" s="3"/>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A234" s="2">
         <v>44880.291912158318</v>
       </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C234" s="3"/>
+      <c r="D234" s="3"/>
+      <c r="E234" s="3"/>
+      <c r="F234" s="3"/>
+      <c r="G234" s="3"/>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A235" s="2">
         <v>44880.312535643578</v>
       </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C235" s="3"/>
+      <c r="D235" s="3"/>
+      <c r="E235" s="3"/>
+      <c r="F235" s="3"/>
+      <c r="G235" s="3"/>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A236" s="2">
         <v>44880.333569566399</v>
       </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C236" s="3"/>
+      <c r="D236" s="3"/>
+      <c r="E236" s="3"/>
+      <c r="F236" s="3"/>
+      <c r="G236" s="3"/>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A237" s="2">
         <v>44880.354206720993</v>
       </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C237" s="3"/>
+      <c r="D237" s="3"/>
+      <c r="E237" s="3"/>
+      <c r="F237" s="3"/>
+      <c r="G237" s="3"/>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A238" s="2">
         <v>44880.375237266213</v>
       </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C238" s="3"/>
+      <c r="D238" s="3"/>
+      <c r="E238" s="3"/>
+      <c r="F238" s="3"/>
+      <c r="G238" s="3"/>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A239" s="2">
         <v>44880.39587338765</v>
       </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C239" s="3"/>
+      <c r="D239" s="3"/>
+      <c r="E239" s="3"/>
+      <c r="F239" s="3"/>
+      <c r="G239" s="3"/>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A240" s="2">
         <v>44880.416910529129</v>
       </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C240" s="3"/>
+      <c r="D240" s="3"/>
+      <c r="E240" s="3"/>
+      <c r="F240" s="3"/>
+      <c r="G240" s="3"/>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A241" s="2">
         <v>44880.437539339073</v>
       </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C241" s="3"/>
+      <c r="D241" s="3"/>
+      <c r="E241" s="3"/>
+      <c r="F241" s="3"/>
+      <c r="G241" s="3"/>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A242" s="2">
         <v>44880.458578467362</v>
       </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C242" s="3"/>
+      <c r="D242" s="3"/>
+      <c r="E242" s="3"/>
+      <c r="F242" s="3"/>
+      <c r="G242" s="3"/>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A243" s="2">
         <v>44880.47920497258</v>
       </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C243" s="3"/>
+      <c r="D243" s="3"/>
+      <c r="E243" s="3"/>
+      <c r="F243" s="3"/>
+      <c r="G243" s="3"/>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A244" s="2">
         <v>44880.500238418579</v>
       </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C244" s="3"/>
+      <c r="D244" s="3"/>
+      <c r="E244" s="3"/>
+      <c r="F244" s="3"/>
+      <c r="G244" s="3"/>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A245" s="2">
         <v>44880.520871758461</v>
       </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C245" s="3"/>
+      <c r="D245" s="3"/>
+      <c r="E245" s="3"/>
+      <c r="F245" s="3"/>
+      <c r="G245" s="3"/>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A246" s="2">
         <v>44880.541904052086</v>
       </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C246" s="3"/>
+      <c r="D246" s="3"/>
+      <c r="E246" s="3"/>
+      <c r="F246" s="3"/>
+      <c r="G246" s="3"/>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A247" s="2">
         <v>44880.562540729843</v>
       </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C247" s="3"/>
+      <c r="D247" s="3"/>
+      <c r="E247" s="3"/>
+      <c r="F247" s="3"/>
+      <c r="G247" s="3"/>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A248" s="2">
         <v>44880.583571632698</v>
       </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C248" s="3"/>
+      <c r="D248" s="3"/>
+      <c r="E248" s="3"/>
+      <c r="F248" s="3"/>
+      <c r="G248" s="3"/>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A249" s="2">
         <v>44880.604206363358</v>
       </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C249" s="3"/>
+      <c r="D249" s="3"/>
+      <c r="E249" s="3"/>
+      <c r="F249" s="3"/>
+      <c r="G249" s="3"/>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A250" s="2">
         <v>44880.625234365463</v>
       </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C250" s="3"/>
+      <c r="D250" s="3"/>
+      <c r="E250" s="3"/>
+      <c r="F250" s="3"/>
+      <c r="G250" s="3"/>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A251" s="2">
         <v>44880.645874420799</v>
       </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C251" s="3"/>
+      <c r="D251" s="3"/>
+      <c r="E251" s="3"/>
+      <c r="F251" s="3"/>
+      <c r="G251" s="3"/>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A252" s="2">
         <v>44880.6669037342</v>
       </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C252" s="3"/>
+      <c r="D252" s="3"/>
+      <c r="E252" s="3"/>
+      <c r="F252" s="3"/>
+      <c r="G252" s="3"/>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A253" s="2">
         <v>44880.687533934914</v>
       </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C253" s="3"/>
+      <c r="D253" s="3"/>
+      <c r="E253" s="3"/>
+      <c r="F253" s="3"/>
+      <c r="G253" s="3"/>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A254" s="2">
         <v>44880.708577871323</v>
       </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C254" s="3"/>
+      <c r="D254" s="3"/>
+      <c r="E254" s="3"/>
+      <c r="F254" s="3"/>
+      <c r="G254" s="3"/>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A255" s="2">
         <v>44880.729203383133</v>
       </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C255" s="3"/>
+      <c r="D255" s="3"/>
+      <c r="E255" s="3"/>
+      <c r="F255" s="3"/>
+      <c r="G255" s="3"/>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A256" s="2">
         <v>44880.75023738543</v>
       </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C256" s="3"/>
+      <c r="D256" s="3"/>
+      <c r="E256" s="3"/>
+      <c r="F256" s="3"/>
+      <c r="G256" s="3"/>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A257" s="2">
         <v>44880.770874420778</v>
       </c>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C257" s="3"/>
+      <c r="D257" s="3"/>
+      <c r="E257" s="3"/>
+      <c r="F257" s="3"/>
+      <c r="G257" s="3"/>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258" s="2">
         <v>44880.791912158318</v>
       </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C258" s="3"/>
+      <c r="D258" s="3"/>
+      <c r="E258" s="3"/>
+      <c r="F258" s="3"/>
+      <c r="G258" s="3"/>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A259" s="2">
         <v>44880.812535206467</v>
       </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C259" s="3"/>
+      <c r="D259" s="3"/>
+      <c r="E259" s="3"/>
+      <c r="F259" s="3"/>
+      <c r="G259" s="3"/>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" s="2">
         <v>44880.833575963967</v>
       </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C260" s="3"/>
+      <c r="D260" s="3"/>
+      <c r="E260" s="3"/>
+      <c r="F260" s="3"/>
+      <c r="G260" s="3"/>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A261" s="2">
         <v>44880.854203621537</v>
       </c>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C261" s="3"/>
+      <c r="D261" s="3"/>
+      <c r="E261" s="3"/>
+      <c r="F261" s="3"/>
+      <c r="G261" s="3"/>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A262" s="2">
         <v>44880.875239610672</v>
       </c>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C262" s="3"/>
+      <c r="D262" s="3"/>
+      <c r="E262" s="3"/>
+      <c r="F262" s="3"/>
+      <c r="G262" s="3"/>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A263" s="2">
         <v>44880.895870288208</v>
       </c>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C263" s="3"/>
+      <c r="D263" s="3"/>
+      <c r="E263" s="3"/>
+      <c r="F263" s="3"/>
+      <c r="G263" s="3"/>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A264" s="2">
         <v>44880.916906118393</v>
       </c>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C264" s="3"/>
+      <c r="D264" s="3"/>
+      <c r="E264" s="3"/>
+      <c r="F264" s="3"/>
+      <c r="G264" s="3"/>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A265" s="2">
         <v>44880.937537272774</v>
       </c>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C265" s="3"/>
+      <c r="D265" s="3"/>
+      <c r="E265" s="3"/>
+      <c r="F265" s="3"/>
+      <c r="G265" s="3"/>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A266" s="2">
         <v>44880.95857834816</v>
       </c>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C266" s="3"/>
+      <c r="D266" s="3"/>
+      <c r="E266" s="3"/>
+      <c r="F266" s="3"/>
+      <c r="G266" s="3"/>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A267" s="2">
         <v>44880.979205767297</v>
       </c>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C267" s="3"/>
+      <c r="D267" s="3"/>
+      <c r="E267" s="3"/>
+      <c r="F267" s="3"/>
+      <c r="G267" s="3"/>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A268" s="2">
         <v>44881.000248263743</v>
       </c>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C268" s="3"/>
+      <c r="D268" s="3"/>
+      <c r="E268" s="3"/>
+      <c r="F268" s="3"/>
+      <c r="G268" s="3"/>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A269" s="2">
         <v>44881.02087303267</v>
       </c>
-    </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C269" s="3"/>
+      <c r="D269" s="3"/>
+      <c r="E269" s="3"/>
+      <c r="F269" s="3"/>
+      <c r="G269" s="3"/>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A270" s="2">
         <v>44881.041908219457</v>
       </c>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C270" s="3"/>
+      <c r="D270" s="3"/>
+      <c r="E270" s="3"/>
+      <c r="F270" s="3"/>
+      <c r="G270" s="3"/>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A271" s="2">
         <v>44881.062536920443</v>
       </c>
-    </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C271" s="3"/>
+      <c r="D271" s="3"/>
+      <c r="E271" s="3"/>
+      <c r="F271" s="3"/>
+      <c r="G271" s="3"/>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A272" s="2">
         <v>44881.083580901213</v>
       </c>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C272" s="3"/>
+      <c r="D272" s="3"/>
+      <c r="E272" s="3"/>
+      <c r="F272" s="3"/>
+      <c r="G272" s="3"/>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A273" s="2">
         <v>44881.104202776478</v>
       </c>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C273" s="3"/>
+      <c r="D273" s="3"/>
+      <c r="E273" s="3"/>
+      <c r="F273" s="3"/>
+      <c r="G273" s="3"/>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A274" s="2">
         <v>44881.125241667018</v>
       </c>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C274" s="3"/>
+      <c r="D274" s="3"/>
+      <c r="E274" s="3"/>
+      <c r="F274" s="3"/>
+      <c r="G274" s="3"/>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A275" s="2">
         <v>44881.145877083138</v>
       </c>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C275" s="3"/>
+      <c r="D275" s="3"/>
+      <c r="E275" s="3"/>
+      <c r="F275" s="3"/>
+      <c r="G275" s="3"/>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A276" s="2">
         <v>44881.16690937677</v>
       </c>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C276" s="3"/>
+      <c r="D276" s="3"/>
+      <c r="E276" s="3"/>
+      <c r="F276" s="3"/>
+      <c r="G276" s="3"/>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A277" s="2">
         <v>44881.187539358922</v>
       </c>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C277" s="3"/>
+      <c r="D277" s="3"/>
+      <c r="E277" s="3"/>
+      <c r="F277" s="3"/>
+      <c r="G277" s="3"/>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A278" s="2">
         <v>44881.208573381104</v>
       </c>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C278" s="3"/>
+      <c r="D278" s="3"/>
+      <c r="E278" s="3"/>
+      <c r="F278" s="3"/>
+      <c r="G278" s="3"/>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A279" s="2">
         <v>44881.229202429437</v>
       </c>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C279" s="3"/>
+      <c r="D279" s="3"/>
+      <c r="E279" s="3"/>
+      <c r="F279" s="3"/>
+      <c r="G279" s="3"/>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A280" s="2">
         <v>44881.250236113869</v>
       </c>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C280" s="3"/>
+      <c r="D280" s="3"/>
+      <c r="E280" s="3"/>
+      <c r="F280" s="3"/>
+      <c r="G280" s="3"/>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A281" s="2">
         <v>44881.270875235386</v>
       </c>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C281" s="3"/>
+      <c r="D281" s="3"/>
+      <c r="E281" s="3"/>
+      <c r="F281" s="3"/>
+      <c r="G281" s="3"/>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A282" s="2">
         <v>44881.291901508957</v>
       </c>
-    </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C282" s="3"/>
+      <c r="D282" s="3"/>
+      <c r="E282" s="3"/>
+      <c r="F282" s="3"/>
+      <c r="G282" s="3"/>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A283" s="2">
         <v>44881.312538186699</v>
       </c>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C283" s="3"/>
+      <c r="D283" s="3"/>
+      <c r="E283" s="3"/>
+      <c r="F283" s="3"/>
+      <c r="G283" s="3"/>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A284" s="2">
         <v>44881.333576043427</v>
       </c>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C284" s="3"/>
+      <c r="D284" s="3"/>
+      <c r="E284" s="3"/>
+      <c r="F284" s="3"/>
+      <c r="G284" s="3"/>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A285" s="2">
         <v>44881.354209621742</v>
       </c>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C285" s="3"/>
+      <c r="D285" s="3"/>
+      <c r="E285" s="3"/>
+      <c r="F285" s="3"/>
+      <c r="G285" s="3"/>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A286" s="2">
         <v>44881.375234842293</v>
       </c>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C286" s="3"/>
+      <c r="D286" s="3"/>
+      <c r="E286" s="3"/>
+      <c r="F286" s="3"/>
+      <c r="G286" s="3"/>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A287" s="2">
         <v>44881.395866195358</v>
       </c>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C287" s="3"/>
+      <c r="D287" s="3"/>
+      <c r="E287" s="3"/>
+      <c r="F287" s="3"/>
+      <c r="G287" s="3"/>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A288" s="2">
         <v>44881.416905562073</v>
       </c>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C288" s="3"/>
+      <c r="D288" s="3"/>
+      <c r="E288" s="3"/>
+      <c r="F288" s="3"/>
+      <c r="G288" s="3"/>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A289" s="2">
         <v>44881.437536358833</v>
       </c>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C289" s="3"/>
+      <c r="D289" s="3"/>
+      <c r="E289" s="3"/>
+      <c r="F289" s="3"/>
+      <c r="G289" s="3"/>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A290" s="2">
         <v>44881.45857139428</v>
       </c>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C290" s="3"/>
+      <c r="D290" s="3"/>
+      <c r="E290" s="3"/>
+      <c r="F290" s="3"/>
+      <c r="G290" s="3"/>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A291" s="2">
         <v>44881.479202429437</v>
       </c>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C291" s="3"/>
+      <c r="D291" s="3"/>
+      <c r="E291" s="3"/>
+      <c r="F291" s="3"/>
+      <c r="G291" s="3"/>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A292" s="2">
         <v>44881.500236113869</v>
       </c>
-    </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C292" s="3"/>
+      <c r="D292" s="3"/>
+      <c r="E292" s="3"/>
+      <c r="F292" s="3"/>
+      <c r="G292" s="3"/>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A293" s="2">
         <v>44881.520871996872</v>
       </c>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C293" s="3"/>
+      <c r="D293" s="3"/>
+      <c r="E293" s="3"/>
+      <c r="F293" s="3"/>
+      <c r="G293" s="3"/>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A294" s="2">
         <v>44881.541903575257</v>
       </c>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C294" s="3"/>
+      <c r="D294" s="3"/>
+      <c r="E294" s="3"/>
+      <c r="F294" s="3"/>
+      <c r="G294" s="3"/>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A295" s="2">
         <v>44881.562540292733</v>
       </c>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C295" s="3"/>
+      <c r="D295" s="3"/>
+      <c r="E295" s="3"/>
+      <c r="F295" s="3"/>
+      <c r="G295" s="3"/>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A296" s="2">
         <v>44881.583570599549</v>
       </c>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C296" s="3"/>
+      <c r="D296" s="3"/>
+      <c r="E296" s="3"/>
+      <c r="F296" s="3"/>
+      <c r="G296" s="3"/>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A297" s="2">
         <v>44881.604201396287</v>
       </c>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C297" s="3"/>
+      <c r="D297" s="3"/>
+      <c r="E297" s="3"/>
+      <c r="F297" s="3"/>
+      <c r="G297" s="3"/>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A298" s="2">
         <v>44881.625241676957</v>
       </c>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C298" s="3"/>
+      <c r="D298" s="3"/>
+      <c r="E298" s="3"/>
+      <c r="F298" s="3"/>
+      <c r="G298" s="3"/>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A299" s="2">
         <v>44881.645876049988</v>
       </c>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C299" s="3"/>
+      <c r="D299" s="3"/>
+      <c r="E299" s="3"/>
+      <c r="F299" s="3"/>
+      <c r="G299" s="3"/>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A300" s="2">
         <v>44881.666907548897</v>
       </c>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C300" s="3"/>
+      <c r="D300" s="3"/>
+      <c r="E300" s="3"/>
+      <c r="F300" s="3"/>
+      <c r="G300" s="3"/>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A301" s="2">
         <v>44881.687532901757</v>
       </c>
-    </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C301" s="3"/>
+      <c r="D301" s="3"/>
+      <c r="E301" s="3"/>
+      <c r="F301" s="3"/>
+      <c r="G301" s="3"/>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A302" s="2">
         <v>44881.708574056618</v>
       </c>
-    </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C302" s="3"/>
+      <c r="D302" s="3"/>
+      <c r="E302" s="3"/>
+      <c r="F302" s="3"/>
+      <c r="G302" s="3"/>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A303" s="2">
         <v>44881.729210058853</v>
       </c>
-    </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C303" s="3"/>
+      <c r="D303" s="3"/>
+      <c r="E303" s="3"/>
+      <c r="F303" s="3"/>
+      <c r="G303" s="3"/>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A304" s="2">
         <v>44881.750236113869</v>
       </c>
-    </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C304" s="3"/>
+      <c r="D304" s="3"/>
+      <c r="E304" s="3"/>
+      <c r="F304" s="3"/>
+      <c r="G304" s="3"/>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A305" s="2">
         <v>44881.770876487091</v>
       </c>
-    </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C305" s="3"/>
+      <c r="D305" s="3"/>
+      <c r="E305" s="3"/>
+      <c r="F305" s="3"/>
+      <c r="G305" s="3"/>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A306" s="2">
         <v>44881.791907787323</v>
       </c>
-    </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C306" s="3"/>
+      <c r="D306" s="3"/>
+      <c r="E306" s="3"/>
+      <c r="F306" s="3"/>
+      <c r="G306" s="3"/>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A307" s="2">
         <v>44881.812539895371</v>
       </c>
-    </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C307" s="3"/>
+      <c r="D307" s="3"/>
+      <c r="E307" s="3"/>
+      <c r="F307" s="3"/>
+      <c r="G307" s="3"/>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A308" s="2">
         <v>44881.833579540253</v>
       </c>
-    </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C308" s="3"/>
+      <c r="D308" s="3"/>
+      <c r="E308" s="3"/>
+      <c r="F308" s="3"/>
+      <c r="G308" s="3"/>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A309" s="2">
         <v>44881.854200204223</v>
       </c>
-    </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C309" s="3"/>
+      <c r="D309" s="3"/>
+      <c r="E309" s="3"/>
+      <c r="F309" s="3"/>
+      <c r="G309" s="3"/>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A310" s="2">
         <v>44881.875238736473</v>
       </c>
-    </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C310" s="3"/>
+      <c r="D310" s="3"/>
+      <c r="E310" s="3"/>
+      <c r="F310" s="3"/>
+      <c r="G310" s="3"/>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A311" s="2">
         <v>44881.895867745079</v>
       </c>
-    </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C311" s="3"/>
+      <c r="D311" s="3"/>
+      <c r="E311" s="3"/>
+      <c r="F311" s="3"/>
+      <c r="G311" s="3"/>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A312" s="2">
         <v>44881.91691374778</v>
       </c>
-    </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C312" s="3"/>
+      <c r="D312" s="3"/>
+      <c r="E312" s="3"/>
+      <c r="F312" s="3"/>
+      <c r="G312" s="3"/>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A313" s="2">
         <v>44881.93753576278</v>
       </c>
-    </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C313" s="3"/>
+      <c r="D313" s="3"/>
+      <c r="E313" s="3"/>
+      <c r="F313" s="3"/>
+      <c r="G313" s="3"/>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A314" s="2">
         <v>44881.958575089768</v>
       </c>
-    </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C314" s="3"/>
+      <c r="D314" s="3"/>
+      <c r="E314" s="3"/>
+      <c r="F314" s="3"/>
+      <c r="G314" s="3"/>
+    </row>
+    <row r="315" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A315" s="2">
         <v>44881.979205210999</v>
       </c>
-    </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C315" s="3"/>
+      <c r="D315" s="3"/>
+      <c r="E315" s="3"/>
+      <c r="F315" s="3"/>
+      <c r="G315" s="3"/>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A316" s="2">
         <v>44882.000241203743</v>
       </c>
-    </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C316" s="3"/>
+      <c r="D316" s="3"/>
+      <c r="E316" s="3"/>
+      <c r="F316" s="3"/>
+      <c r="G316" s="3"/>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A317" s="2">
         <v>44882.020868403379</v>
       </c>
-    </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C317" s="3"/>
+      <c r="D317" s="3"/>
+      <c r="E317" s="3"/>
+      <c r="F317" s="3"/>
+      <c r="G317" s="3"/>
+    </row>
+    <row r="318" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A318" s="2">
         <v>44882.041914234549</v>
       </c>
-    </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C318" s="3"/>
+      <c r="D318" s="3"/>
+      <c r="E318" s="3"/>
+      <c r="F318" s="3"/>
+      <c r="G318" s="3"/>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A319" s="2">
         <v>44882.062536920443</v>
       </c>
-    </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C319" s="3"/>
+      <c r="D319" s="3"/>
+      <c r="E319" s="3"/>
+      <c r="F319" s="3"/>
+      <c r="G319" s="3"/>
+    </row>
+    <row r="320" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A320" s="2">
         <v>44882.083576848097</v>
       </c>
-    </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C320" s="3"/>
+      <c r="D320" s="3"/>
+      <c r="E320" s="3"/>
+      <c r="F320" s="3"/>
+      <c r="G320" s="3"/>
+    </row>
+    <row r="321" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A321" s="2">
         <v>44882.104210416474</v>
       </c>
-    </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C321" s="3"/>
+      <c r="D321" s="3"/>
+      <c r="E321" s="3"/>
+      <c r="F321" s="3"/>
+      <c r="G321" s="3"/>
+    </row>
+    <row r="322" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A322" s="2">
         <v>44882.12524444858</v>
       </c>
-    </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C322" s="3"/>
+      <c r="D322" s="3"/>
+      <c r="E322" s="3"/>
+      <c r="F322" s="3"/>
+      <c r="G322" s="3"/>
+    </row>
+    <row r="323" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A323" s="2">
         <v>44882.145868052372</v>
       </c>
-    </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C323" s="3"/>
+      <c r="D323" s="3"/>
+      <c r="E323" s="3"/>
+      <c r="F323" s="3"/>
+      <c r="G323" s="3"/>
+    </row>
+    <row r="324" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A324" s="2">
         <v>44882.166914244488</v>
       </c>
-    </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C324" s="3"/>
+      <c r="D324" s="3"/>
+      <c r="E324" s="3"/>
+      <c r="F324" s="3"/>
+      <c r="G324" s="3"/>
+    </row>
+    <row r="325" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A325" s="2">
         <v>44882.187538882092</v>
       </c>
-    </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C325" s="3"/>
+      <c r="D325" s="3"/>
+      <c r="E325" s="3"/>
+      <c r="F325" s="3"/>
+      <c r="G325" s="3"/>
+    </row>
+    <row r="326" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A326" s="2">
         <v>44882.208568394177</v>
       </c>
-    </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C326" s="3"/>
+      <c r="D326" s="3"/>
+      <c r="E326" s="3"/>
+      <c r="F326" s="3"/>
+      <c r="G326" s="3"/>
+    </row>
+    <row r="327" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A327" s="2">
         <v>44882.229201614849</v>
       </c>
-    </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C327" s="3"/>
+      <c r="D327" s="3"/>
+      <c r="E327" s="3"/>
+      <c r="F327" s="3"/>
+      <c r="G327" s="3"/>
+    </row>
+    <row r="328" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A328" s="2">
         <v>44882.25024698177</v>
       </c>
-    </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C328" s="3"/>
+      <c r="D328" s="3"/>
+      <c r="E328" s="3"/>
+      <c r="F328" s="3"/>
+      <c r="G328" s="3"/>
+    </row>
+    <row r="329" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A329" s="2">
         <v>44882.270872215428</v>
       </c>
-    </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C329" s="3"/>
+      <c r="D329" s="3"/>
+      <c r="E329" s="3"/>
+      <c r="F329" s="3"/>
+      <c r="G329" s="3"/>
+    </row>
+    <row r="330" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A330" s="2">
         <v>44882.291911919907</v>
       </c>
-    </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C330" s="3"/>
+      <c r="D330" s="3"/>
+      <c r="E330" s="3"/>
+      <c r="F330" s="3"/>
+      <c r="G330" s="3"/>
+    </row>
+    <row r="331" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A331" s="2">
         <v>44882.31253576278</v>
       </c>
-    </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C331" s="3"/>
+      <c r="D331" s="3"/>
+      <c r="E331" s="3"/>
+      <c r="F331" s="3"/>
+      <c r="G331" s="3"/>
+    </row>
+    <row r="332" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A332" s="2">
         <v>44882.333571513482</v>
       </c>
-    </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C332" s="3"/>
+      <c r="D332" s="3"/>
+      <c r="E332" s="3"/>
+      <c r="F332" s="3"/>
+      <c r="G332" s="3"/>
+    </row>
+    <row r="333" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A333" s="2">
         <v>44882.354205449417</v>
       </c>
-    </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C333" s="3"/>
+      <c r="D333" s="3"/>
+      <c r="E333" s="3"/>
+      <c r="F333" s="3"/>
+      <c r="G333" s="3"/>
+    </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A334" s="2">
         <v>44882.375242590897</v>
       </c>
-    </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C334" s="3"/>
+      <c r="D334" s="3"/>
+      <c r="E334" s="3"/>
+      <c r="F334" s="3"/>
+      <c r="G334" s="3"/>
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A335" s="2">
         <v>44882.395866552972</v>
       </c>
-    </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C335" s="3"/>
+      <c r="D335" s="3"/>
+      <c r="E335" s="3"/>
+      <c r="F335" s="3"/>
+      <c r="G335" s="3"/>
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A336" s="2">
         <v>44882.416912277527</v>
       </c>
-    </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C336" s="3"/>
+      <c r="D336" s="3"/>
+      <c r="E336" s="3"/>
+      <c r="F336" s="3"/>
+      <c r="G336" s="3"/>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A337" s="2">
         <v>44882.43753369648</v>
       </c>
-    </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C337" s="3"/>
+      <c r="D337" s="3"/>
+      <c r="E337" s="3"/>
+      <c r="F337" s="3"/>
+      <c r="G337" s="3"/>
+    </row>
+    <row r="338" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A338" s="2">
         <v>44882.458567380912</v>
       </c>
-    </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C338" s="3"/>
+      <c r="D338" s="3"/>
+      <c r="E338" s="3"/>
+      <c r="F338" s="3"/>
+      <c r="G338" s="3"/>
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A339" s="2">
         <v>44882.479203343391</v>
       </c>
-    </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C339" s="3"/>
+      <c r="D339" s="3"/>
+      <c r="E339" s="3"/>
+      <c r="F339" s="3"/>
+      <c r="G339" s="3"/>
+    </row>
+    <row r="340" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A340" s="2">
         <v>44882.500234047569</v>
       </c>
-    </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C340" s="3"/>
+      <c r="D340" s="3"/>
+      <c r="E340" s="3"/>
+      <c r="F340" s="3"/>
+      <c r="G340" s="3"/>
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A341" s="2">
         <v>44882.520871996872</v>
       </c>
-    </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C341" s="3"/>
+      <c r="D341" s="3"/>
+      <c r="E341" s="3"/>
+      <c r="F341" s="3"/>
+      <c r="G341" s="3"/>
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A342" s="2">
         <v>44882.541901866593</v>
       </c>
-    </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C342" s="3"/>
+      <c r="D342" s="3"/>
+      <c r="E342" s="3"/>
+      <c r="F342" s="3"/>
+      <c r="G342" s="3"/>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A343" s="2">
         <v>44882.562536358833</v>
       </c>
-    </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C343" s="3"/>
+      <c r="D343" s="3"/>
+      <c r="E343" s="3"/>
+      <c r="F343" s="3"/>
+      <c r="G343" s="3"/>
+    </row>
+    <row r="344" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A344" s="2">
         <v>44882.583576162651</v>
       </c>
-    </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C344" s="3"/>
+      <c r="D344" s="3"/>
+      <c r="E344" s="3"/>
+      <c r="F344" s="3"/>
+      <c r="G344" s="3"/>
+    </row>
+    <row r="345" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A345" s="2">
         <v>44882.604204853371</v>
       </c>
-    </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C345" s="3"/>
+      <c r="D345" s="3"/>
+      <c r="E345" s="3"/>
+      <c r="F345" s="3"/>
+      <c r="G345" s="3"/>
+    </row>
+    <row r="346" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A346" s="2">
         <v>44882.625244458497</v>
       </c>
-    </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C346" s="3"/>
+      <c r="D346" s="3"/>
+      <c r="E346" s="3"/>
+      <c r="F346" s="3"/>
+      <c r="G346" s="3"/>
+    </row>
+    <row r="347" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A347" s="2">
         <v>44882.645873943948</v>
       </c>
-    </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C347" s="3"/>
+      <c r="D347" s="3"/>
+      <c r="E347" s="3"/>
+      <c r="F347" s="3"/>
+      <c r="G347" s="3"/>
+    </row>
+    <row r="348" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A348" s="2">
         <v>44882.666909297302</v>
       </c>
-    </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C348" s="3"/>
+      <c r="D348" s="3"/>
+      <c r="E348" s="3"/>
+      <c r="F348" s="3"/>
+      <c r="G348" s="3"/>
+    </row>
+    <row r="349" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A349" s="2">
         <v>44882.687541007988</v>
       </c>
-    </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C349" s="3"/>
+      <c r="D349" s="3"/>
+      <c r="E349" s="3"/>
+      <c r="F349" s="3"/>
+      <c r="G349" s="3"/>
+    </row>
+    <row r="350" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A350" s="2">
         <v>44882.708570400871</v>
       </c>
-    </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C350" s="3"/>
+      <c r="D350" s="3"/>
+      <c r="E350" s="3"/>
+      <c r="F350" s="3"/>
+      <c r="G350" s="3"/>
+    </row>
+    <row r="351" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A351" s="2">
         <v>44882.72920497258</v>
       </c>
-    </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C351" s="3"/>
+      <c r="D351" s="3"/>
+      <c r="E351" s="3"/>
+      <c r="F351" s="3"/>
+      <c r="G351" s="3"/>
+    </row>
+    <row r="352" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A352" s="2">
         <v>44882.750241756432</v>
       </c>
-    </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C352" s="3"/>
+      <c r="D352" s="3"/>
+      <c r="E352" s="3"/>
+      <c r="F352" s="3"/>
+      <c r="G352" s="3"/>
+    </row>
+    <row r="353" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A353" s="2">
         <v>44882.770871798202</v>
       </c>
-    </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C353" s="3"/>
+      <c r="D353" s="3"/>
+      <c r="E353" s="3"/>
+      <c r="F353" s="3"/>
+      <c r="G353" s="3"/>
+    </row>
+    <row r="354" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A354" s="2">
         <v>44882.791910648353</v>
       </c>
-    </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C354" s="3"/>
+      <c r="D354" s="3"/>
+      <c r="E354" s="3"/>
+      <c r="F354" s="3"/>
+      <c r="G354" s="3"/>
+    </row>
+    <row r="355" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A355" s="2">
         <v>44882.812533775948</v>
       </c>
+      <c r="C355" s="3"/>
+      <c r="D355" s="3"/>
+      <c r="E355" s="3"/>
+      <c r="F355" s="3"/>
+      <c r="G355" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>